<commit_message>
seed dummy data 955
</commit_message>
<xml_diff>
--- a/public/DatabaseRecovery/sql/Rekap Data Rental Mobil.xlsx
+++ b/public/DatabaseRecovery/sql/Rekap Data Rental Mobil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PNL\MK\Tugas Akhir\TGA-Code\tga-rental-mobil\public\DatabaseRecovery\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D11BDC4-4B2A-474A-8CA2-9DB75D4657F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C035A300-81C5-4A1F-95DF-5E13D1CB0C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{0FFBED60-907F-4311-94AD-12BB782D49C3}"/>
+    <workbookView xWindow="-7005" yWindow="0" windowWidth="15375" windowHeight="7995" firstSheet="2" activeTab="2" xr2:uid="{0FFBED60-907F-4311-94AD-12BB782D49C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Akun" sheetId="1" r:id="rId1"/>
@@ -1122,7 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A976FF88-3BA2-4D47-8A1E-61292A7499DC}">
   <dimension ref="E4:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1389,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F89D9F5-B1D6-48D1-930D-6DBF8F6F234E}">
   <dimension ref="C4:M113"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M73" sqref="M73"/>
+    <sheetView tabSelected="1" topLeftCell="F24" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4623,8 +4623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A72435-518D-40D4-88A4-F9FACB9974C4}">
   <dimension ref="A1:P903"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="B46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>